<commit_message>
se corrige para que no cambie los combos en riesgos eventos e incidentes
</commit_message>
<xml_diff>
--- a/ListasSarlaft/BDupdate/CambiosBD_V2.xlsx
+++ b/ListasSarlaft/BDupdate/CambiosBD_V2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\OneDrive - 848096_1398524_DATALAFT_SAS\Escritorio\shercklock_ficohsa\Sherlock_V5\ListasSarlaft\BDupdate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Desktop\sherlock_ficohsa\SherlockFicohsa_Pro\ListasSarlaft\BDupdate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E2CD419-DDFC-42E3-9FE9-8CFCE470BB02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46C98B80-671F-4852-AE23-0634D072A884}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -7725,8 +7725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J281"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A268" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A278" sqref="A278"/>
+    <sheetView tabSelected="1" topLeftCell="A273" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E279" sqref="E279"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>